<commit_message>
Ogranicen broj pitanja na 10
</commit_message>
<xml_diff>
--- a/data/Participants.xlsx
+++ b/data/Participants.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t>Ime</t>
   </si>
@@ -31,12 +31,145 @@
   </si>
   <si>
     <t>Broj poena</t>
+  </si>
+  <si>
+    <t>jeca</t>
+  </si>
+  <si>
+    <t>milev</t>
+  </si>
+  <si>
+    <t>kdkdljfs</t>
+  </si>
+  <si>
+    <t>lkfdsf</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>ghsd</t>
+  </si>
+  <si>
+    <t>kjsdksjd</t>
+  </si>
+  <si>
+    <t>snjksjd</t>
+  </si>
+  <si>
+    <t>skksjds</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>fg</t>
+  </si>
+  <si>
+    <t>gsfg</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>cvc</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>lkj</t>
+  </si>
+  <si>
+    <t>ljlj</t>
+  </si>
+  <si>
+    <t>ljlkj</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>jujhg</t>
+  </si>
+  <si>
+    <t>jg</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>sfs</t>
+  </si>
+  <si>
+    <t>dfg</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>jh</t>
+  </si>
+  <si>
+    <t>jhj</t>
+  </si>
+  <si>
+    <t>jhjh</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>fdg</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sd</t>
+  </si>
+  <si>
+    <t>af</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>sdg</t>
+  </si>
+  <si>
+    <t>dg</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>xh</t>
+  </si>
+  <si>
+    <t>dfh</t>
+  </si>
+  <si>
+    <t>fgh</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -373,7 +506,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E2"/>
@@ -396,6 +529,210 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Promenjen efekat za prikaz pitanja na fade in
</commit_message>
<xml_diff>
--- a/data/Participants.xlsx
+++ b/data/Participants.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="118">
   <si>
     <t>Ime</t>
   </si>
@@ -163,6 +163,213 @@
   </si>
   <si>
     <t>11</t>
+  </si>
+  <si>
+    <t>sgs</t>
+  </si>
+  <si>
+    <t>dfgf</t>
+  </si>
+  <si>
+    <t>gvsg</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>dfgdgd</t>
+  </si>
+  <si>
+    <t>gdfg</t>
+  </si>
+  <si>
+    <t>dgdfg</t>
+  </si>
+  <si>
+    <t>dfgdf</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>sdfsd</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>sfg</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>sdfg</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>dasf</t>
+  </si>
+  <si>
+    <t>dsf</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>vvcx</t>
+  </si>
+  <si>
+    <t>xcv</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sddf</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> df</t>
+  </si>
+  <si>
+    <t>sdfs</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>adf</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>sdaf</t>
+  </si>
+  <si>
+    <t>sdv</t>
+  </si>
+  <si>
+    <t>cxvxcv</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>dsvsd</t>
+  </si>
+  <si>
+    <t>kh</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>hf</t>
+  </si>
+  <si>
+    <t>bnf</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>dfs</t>
+  </si>
+  <si>
+    <t>sf</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v </t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>hh</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> jJj</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> j</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> h</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>hg</t>
+  </si>
+  <si>
+    <t>j`j`j`j`</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>ldjkLX</t>
+  </si>
+  <si>
+    <t>x.vm.</t>
+  </si>
+  <si>
+    <t>.CVM</t>
   </si>
 </sst>
 </file>
@@ -506,7 +713,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E2"/>
@@ -733,6 +940,805 @@
       </c>
       <c r="E13" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" t="s">
+        <v>98</v>
+      </c>
+      <c r="E37" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" t="s">
+        <v>91</v>
+      </c>
+      <c r="E38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>99</v>
+      </c>
+      <c r="B39" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" t="s">
+        <v>91</v>
+      </c>
+      <c r="E40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" t="s">
+        <v>101</v>
+      </c>
+      <c r="E41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" t="s">
+        <v>103</v>
+      </c>
+      <c r="D42" t="s">
+        <v>103</v>
+      </c>
+      <c r="E42" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43" t="s">
+        <v>101</v>
+      </c>
+      <c r="E43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>104</v>
+      </c>
+      <c r="B44" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" t="s">
+        <v>101</v>
+      </c>
+      <c r="D44" t="s">
+        <v>101</v>
+      </c>
+      <c r="E44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" t="s">
+        <v>103</v>
+      </c>
+      <c r="C45" t="s">
+        <v>103</v>
+      </c>
+      <c r="D45" t="s">
+        <v>103</v>
+      </c>
+      <c r="E45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" t="s">
+        <v>103</v>
+      </c>
+      <c r="D46" t="s">
+        <v>103</v>
+      </c>
+      <c r="E46" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>108</v>
+      </c>
+      <c r="B47" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" t="s">
+        <v>101</v>
+      </c>
+      <c r="E47" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>103</v>
+      </c>
+      <c r="B48" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" t="s">
+        <v>103</v>
+      </c>
+      <c r="E48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" t="s">
+        <v>101</v>
+      </c>
+      <c r="D49" t="s">
+        <v>101</v>
+      </c>
+      <c r="E49" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50" t="s">
+        <v>26</v>
+      </c>
+      <c r="E50" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51" t="s">
+        <v>103</v>
+      </c>
+      <c r="D51" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52" t="s">
+        <v>110</v>
+      </c>
+      <c r="E52" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" t="s">
+        <v>103</v>
+      </c>
+      <c r="D53" t="s">
+        <v>103</v>
+      </c>
+      <c r="E53" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" t="s">
+        <v>103</v>
+      </c>
+      <c r="E54" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>104</v>
+      </c>
+      <c r="B55" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" t="s">
+        <v>104</v>
+      </c>
+      <c r="D55" t="s">
+        <v>104</v>
+      </c>
+      <c r="E55" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>112</v>
+      </c>
+      <c r="B56" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" t="s">
+        <v>112</v>
+      </c>
+      <c r="D56" t="s">
+        <v>26</v>
+      </c>
+      <c r="E56" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>113</v>
+      </c>
+      <c r="B57" t="s">
+        <v>113</v>
+      </c>
+      <c r="C57" t="s">
+        <v>113</v>
+      </c>
+      <c r="D57" t="s">
+        <v>113</v>
+      </c>
+      <c r="E57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>108</v>
+      </c>
+      <c r="B58" t="s">
+        <v>101</v>
+      </c>
+      <c r="C58" t="s">
+        <v>101</v>
+      </c>
+      <c r="D58" t="s">
+        <v>101</v>
+      </c>
+      <c r="E58" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" t="s">
+        <v>103</v>
+      </c>
+      <c r="C59" t="s">
+        <v>103</v>
+      </c>
+      <c r="D59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E59" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>115</v>
+      </c>
+      <c r="B60" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60" t="s">
+        <v>117</v>
+      </c>
+      <c r="D60" t="s">
+        <v>26</v>
+      </c>
+      <c r="E60" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dodat ispis poruke sa brojem osvojenih poena
</commit_message>
<xml_diff>
--- a/data/Participants.xlsx
+++ b/data/Participants.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="127">
   <si>
     <t>Ime</t>
   </si>
@@ -370,6 +370,33 @@
   </si>
   <si>
     <t>.CVM</t>
+  </si>
+  <si>
+    <t>afkjl</t>
+  </si>
+  <si>
+    <t>smv</t>
+  </si>
+  <si>
+    <t>ksdm</t>
+  </si>
+  <si>
+    <t>cxv</t>
+  </si>
+  <si>
+    <t>fdgdfg</t>
+  </si>
+  <si>
+    <t>xv</t>
+  </si>
+  <si>
+    <t>xcx</t>
+  </si>
+  <si>
+    <t>xb</t>
+  </si>
+  <si>
+    <t>vcb</t>
   </si>
 </sst>
 </file>
@@ -713,7 +740,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E2"/>
@@ -1739,6 +1766,91 @@
       </c>
       <c r="E60" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61" t="s">
+        <v>120</v>
+      </c>
+      <c r="D61" t="s">
+        <v>121</v>
+      </c>
+      <c r="E61" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" t="s">
+        <v>29</v>
+      </c>
+      <c r="C62" t="s">
+        <v>36</v>
+      </c>
+      <c r="D62" t="s">
+        <v>29</v>
+      </c>
+      <c r="E62" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>97</v>
+      </c>
+      <c r="B63" t="s">
+        <v>97</v>
+      </c>
+      <c r="C63" t="s">
+        <v>123</v>
+      </c>
+      <c r="D63" t="s">
+        <v>26</v>
+      </c>
+      <c r="E63" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>91</v>
+      </c>
+      <c r="B64" t="s">
+        <v>124</v>
+      </c>
+      <c r="C64" t="s">
+        <v>125</v>
+      </c>
+      <c r="D64" t="s">
+        <v>26</v>
+      </c>
+      <c r="E64" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>42</v>
+      </c>
+      <c r="B65" t="s">
+        <v>125</v>
+      </c>
+      <c r="C65" t="s">
+        <v>126</v>
+      </c>
+      <c r="D65" t="s">
+        <v>26</v>
+      </c>
+      <c r="E65" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Encoding for reading questions added
</commit_message>
<xml_diff>
--- a/data/Participants.xlsx
+++ b/data/Participants.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Ime</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>6</t>
+  </si>
+  <si>
+    <t>dzeca</t>
+  </si>
+  <si>
+    <t>dzeca@gmail</t>
+  </si>
+  <si>
+    <t>;sd;fklad;klf</t>
+  </si>
+  <si>
+    <t>20</t>
   </si>
 </sst>
 </file>
@@ -413,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
@@ -494,6 +506,23 @@
         <v>17</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>